<commit_message>
testing different options, last test is PedroCV. The vitae package looks unstable
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,26 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\cv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4678EEBE-83A1-4798-B90D-19C6D0E4C6EA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B18065-3C6C-4BCA-A7F9-19793D933711}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="awards" sheetId="1" r:id="rId1"/>
-    <sheet name="work-experience" sheetId="3" r:id="rId2"/>
-    <sheet name="testw" sheetId="2" r:id="rId3"/>
+    <sheet name="config" sheetId="4" r:id="rId1"/>
+    <sheet name="education" sheetId="7" r:id="rId2"/>
+    <sheet name="awards" sheetId="1" r:id="rId3"/>
+    <sheet name="work-experience" sheetId="3" r:id="rId4"/>
+    <sheet name="testw" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="70">
   <si>
     <t>Source</t>
   </si>
@@ -94,6 +102,153 @@
   </si>
   <si>
     <t>Company</t>
+  </si>
+  <si>
+    <t>Lecturer</t>
+  </si>
+  <si>
+    <t>2018 - 2019</t>
+  </si>
+  <si>
+    <t>Section</t>
+  </si>
+  <si>
+    <t>Include</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>brief</t>
+  </si>
+  <si>
+    <t>Work</t>
+  </si>
+  <si>
+    <t>Awards</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>SoftwareSkills</t>
+  </si>
+  <si>
+    <t>Activities</t>
+  </si>
+  <si>
+    <t>Projects</t>
+  </si>
+  <si>
+    <t>Presentations</t>
+  </si>
+  <si>
+    <t>Books</t>
+  </si>
+  <si>
+    <t>JournalPapers</t>
+  </si>
+  <si>
+    <t>Dissertations</t>
+  </si>
+  <si>
+    <t>bib</t>
+  </si>
+  <si>
+    <t>Master Research Assistant</t>
+  </si>
+  <si>
+    <t>2016 - 2018</t>
+  </si>
+  <si>
+    <t>Undergraduate Research Intern</t>
+  </si>
+  <si>
+    <t>2013 - 2015</t>
+  </si>
+  <si>
+    <t>UNISINOS University, Brazil</t>
+  </si>
+  <si>
+    <t>Rede Industrial, Brazil</t>
+  </si>
+  <si>
+    <t>Chief Analyst</t>
+  </si>
+  <si>
+    <t>2012 - 2013</t>
+  </si>
+  <si>
+    <t>Business Analyst</t>
+  </si>
+  <si>
+    <t>2009 - 2012</t>
+  </si>
+  <si>
+    <t>Support Assistant</t>
+  </si>
+  <si>
+    <t>2008 - 2009</t>
+  </si>
+  <si>
+    <t>Carried out requirement and use-case analysis for software improvements; Developed a working knowledge of Structured Query Language (SQL) for database reporting.</t>
+  </si>
+  <si>
+    <t>Oversaw SIGMA's (a computerized maintenance management software) development and support teams.</t>
+  </si>
+  <si>
+    <t>Provided assistantship for research projects delivered to private companies and public agencies. Developed an interface for system dynamics simulation integrating Ithink software and Excel, using VBA.</t>
+  </si>
+  <si>
+    <t>Developed a Monte Carlo Simulation package in R for cost-benefit analysis of Organizational Safety and Health Initiatives. In the scope of the master's research project, developed a range of algorithms for exploratory modeling and analysis of system dynamics models in R, using the Robust Decision Making approach.</t>
+  </si>
+  <si>
+    <t>Served as a Lecturer for Undergraduate and MBE courses in the Industrial Engineering Department. Disciplines: Operations Research - Linear Programming; Simulation Modeling (Discrete Event Simulation);  System Dynamics Simulation. Operations Management; Information Systems Management.</t>
+  </si>
+  <si>
+    <t>Assisted Sigma’s customers’ issues troubleshooting and Sigma’s Quality Assurance processes.</t>
+  </si>
+  <si>
+    <t>RAND Corporation, US</t>
+  </si>
+  <si>
+    <t>Policy Research Assistant</t>
+  </si>
+  <si>
+    <t>Provides assistantship to research projects undertaken at RAND Corporation.</t>
+  </si>
+  <si>
+    <t>Ph.D. in Policy Analysis</t>
+  </si>
+  <si>
+    <t>B.Sc. in Production Engineering</t>
+  </si>
+  <si>
+    <t>2009 - 2015</t>
+  </si>
+  <si>
+    <t>M.Sc. in Production Engineering</t>
+  </si>
+  <si>
+    <t>2019 - current</t>
+  </si>
+  <si>
+    <t>School</t>
+  </si>
+  <si>
+    <t>Pardee RAND Graduate School, CA, U.S.</t>
+  </si>
+  <si>
+    <t>2019 - 202X</t>
   </si>
 </sst>
 </file>
@@ -413,12 +568,241 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EB30E6B-3E82-4828-871F-0130ED3058AE}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1AD67A5-C15E-466B-AB72-CEFC2B3717C0}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="56" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="4" max="4" width="71.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -516,18 +900,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C533C8A3-9B8F-4D5E-80C3-E035B1F1AAB2}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="128.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -545,74 +930,102 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>2018</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>2016</v>
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>2016</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5">
-        <v>2015</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6">
-        <v>2013</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
+        <v>47</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -620,7 +1033,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6811A89-14BC-4952-A431-37EAD9A13ECA}">
   <dimension ref="A1:C2"/>
   <sheetViews>

</xml_diff>